<commit_message>
Fixed errors in Excel exercises.
</commit_message>
<xml_diff>
--- a/formulas/autocarsa.xlsx
+++ b/formulas/autocarsa.xlsx
@@ -51,9 +51,6 @@
     <t>Cars</t>
   </si>
   <si>
-    <t>Motocycles</t>
-  </si>
-  <si>
     <t>Registration tax</t>
   </si>
   <si>
@@ -101,6 +98,9 @@
   <si>
     <t>%VAT</t>
   </si>
+  <si>
+    <t>Motorcycles</t>
+  </si>
 </sst>
 </file>
 
@@ -108,7 +108,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-[$€-2]\ * #,##0_-;\-[$€-2]\ * #,##0_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0_-;\-[$€-2]\ * #,##0_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -218,16 +218,13 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -244,6 +241,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,50 +554,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -616,10 +616,10 @@
       <c r="E3" s="4">
         <v>12</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -637,10 +637,10 @@
       <c r="E4" s="5">
         <v>8</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -658,14 +658,14 @@
       <c r="E5" s="5">
         <v>30</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7">
         <v>10</v>
@@ -679,62 +679,62 @@
       <c r="E6" s="7">
         <v>6</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+        <v>14</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="18"/>
+        <v>10</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
+        <v>12</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -755,7 +755,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -764,43 +764,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="A1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -819,19 +819,19 @@
       <c r="E3" s="4">
         <v>11</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <f>SUM(B3:E3)*Prices!B2</f>
         <v>1020000</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <f>F3*Taxes!B2</f>
         <v>99450</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <f>F3*Taxes!B$8</f>
         <v>214200</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="9">
         <f>SUM(F3:H3)</f>
         <v>1333650</v>
       </c>
@@ -852,19 +852,19 @@
       <c r="E4" s="5">
         <v>5</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <f>SUM(B4:E4)*Prices!B3</f>
         <v>770000</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <f>F4*Taxes!B3</f>
         <v>113575</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <f>F4*Taxes!B$8</f>
         <v>161700</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="10">
         <f t="shared" ref="I4:I6" si="0">SUM(F4:H4)</f>
         <v>1045275</v>
       </c>
@@ -885,26 +885,26 @@
       <c r="E5" s="5">
         <v>15</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f>SUM(B5:E5)*Prices!B4</f>
         <v>1701000</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <f>F5*Taxes!B4</f>
         <v>165847.5</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <f>F5*Taxes!B$8</f>
         <v>357210</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <f t="shared" si="0"/>
         <v>2224057.5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7">
         <v>6</v>
@@ -918,131 +918,131 @@
       <c r="E6" s="7">
         <v>3</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f>SUM(B6:E6)*Prices!B5</f>
         <v>210000</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <f>F6*Taxes!B5</f>
         <v>9975</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f>F6*Taxes!B$8</f>
         <v>44100</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <f t="shared" si="0"/>
         <v>264075</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="11">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10">
         <f>B3*Prices!$B2+B4*Prices!$B3+B5*Prices!$B4+B6*Prices!$B5</f>
         <v>1025000</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <f>C3*Prices!$B2+C4*Prices!$B3+C5*Prices!$B4+C6*Prices!$B5</f>
         <v>1073000</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <f>D3*Prices!$B2+D4*Prices!$B3+D5*Prices!$B4+D6*Prices!$B5</f>
         <v>925500</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <f>E3*Prices!$B2+E4*Prices!$B3+E5*Prices!$B4+E6*Prices!$B5</f>
         <v>677500</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <f>SUM(F3:F6)</f>
         <v>3701000</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="11">
+        <v>14</v>
+      </c>
+      <c r="B8" s="10">
         <f>B3*Prices!$B2*Taxes!$B2+B4*Prices!$B3*Taxes!$B3+B5*Prices!$B4*Taxes!$B4+B6*Prices!$B5*Taxes!$B5</f>
         <v>104687.5</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <f>C3*Prices!$B2*Taxes!$B2+C4*Prices!$B3*Taxes!$B3+C5*Prices!$B4*Taxes!$B4+C6*Prices!$B5*Taxes!$B5</f>
         <v>112367.5</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <f>D3*Prices!$B2*Taxes!$B2+D4*Prices!$B3*Taxes!$B3+D5*Prices!$B4*Taxes!$B4+D6*Prices!$B5*Taxes!$B5</f>
         <v>98111.25</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <f>E3*Prices!$B2*Taxes!$B2+E4*Prices!$B3*Taxes!$B3+E5*Prices!$B4*Taxes!$B4+E6*Prices!$B5*Taxes!$B5</f>
         <v>73681.25</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12">
+      <c r="F8" s="10"/>
+      <c r="G8" s="11">
         <f>SUM(G3:G6)</f>
         <v>388847.5</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="11">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10">
         <f>B7*Taxes!$B8</f>
         <v>215250</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <f>C7*Taxes!$B8</f>
         <v>225330</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <f>D7*Taxes!$B8</f>
         <v>194355</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <f>E7*Taxes!$B8</f>
         <v>142275</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11">
         <f>SUM(H3:H6)</f>
         <v>777210</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="13">
+        <v>12</v>
+      </c>
+      <c r="B10" s="12">
         <f>SUM(B7:B9)</f>
         <v>1344937.5</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <f t="shared" ref="C10:E10" si="1">SUM(C7:C9)</f>
         <v>1410697.5</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <f t="shared" si="1"/>
         <v>1217966.25</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <f t="shared" si="1"/>
         <v>893456.25</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13">
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12">
         <f>SUM(I3:I6)</f>
         <v>4867057.5</v>
       </c>
@@ -1066,50 +1066,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="A1" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1128,19 +1128,19 @@
       <c r="E3" s="4">
         <v>16</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <f>SUM(B3:E3)*Prices!B2</f>
         <v>825000</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <f>F3*Taxes!B2</f>
         <v>80437.5</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <f>F3*Taxes!B$8</f>
         <v>173250</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="9">
         <f>SUM(F3:H3)</f>
         <v>1078687.5</v>
       </c>
@@ -1161,19 +1161,19 @@
       <c r="E4" s="5">
         <v>8</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <f>SUM(B4:E4)*Prices!B3</f>
         <v>805000</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <f>F4*Taxes!B3</f>
         <v>118737.5</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <f>F4*Taxes!B$8</f>
         <v>169050</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="10">
         <f t="shared" ref="I4:I6" si="0">SUM(F4:H4)</f>
         <v>1092787.5</v>
       </c>
@@ -1194,26 +1194,26 @@
       <c r="E5" s="5">
         <v>41</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f>SUM(B5:E5)*Prices!B4</f>
         <v>3255000</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <f>F5*Taxes!B4</f>
         <v>317362.5</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <f>F5*Taxes!B$8</f>
         <v>683550</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <f t="shared" si="0"/>
         <v>4255912.5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7">
         <v>14</v>
@@ -1227,131 +1227,131 @@
       <c r="E6" s="7">
         <v>15</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f>SUM(B6:E6)*Prices!B5</f>
         <v>607500</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <f>F6*Taxes!B5</f>
         <v>28856.25</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f>F6*Taxes!B$8</f>
         <v>127575</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <f t="shared" si="0"/>
         <v>763931.25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="11">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10">
         <f>B3*Prices!$B2+B4*Prices!$B3+B5*Prices!$B4+B6*Prices!$B5</f>
         <v>1237000</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <f>C3*Prices!$B2+C4*Prices!$B3+C5*Prices!$B4+C6*Prices!$B5</f>
         <v>1248500</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <f>D3*Prices!$B2+D4*Prices!$B3+D5*Prices!$B4+D6*Prices!$B5</f>
         <v>1513500</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <f>E3*Prices!$B2+E4*Prices!$B3+E5*Prices!$B4+E6*Prices!$B5</f>
         <v>1493500</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <f>SUM(F3:F6)</f>
         <v>5492500</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="11">
+        <v>14</v>
+      </c>
+      <c r="B8" s="10">
         <f>B3*Prices!$B2*Taxes!$B2+B4*Prices!$B3*Taxes!$B3+B5*Prices!$B4*Taxes!$B4+B6*Prices!$B5*Taxes!$B5</f>
         <v>129357.5</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <f>C3*Prices!$B2*Taxes!$B2+C4*Prices!$B3*Taxes!$B3+C5*Prices!$B4*Taxes!$B4+C6*Prices!$B5*Taxes!$B5</f>
         <v>120103.75</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <f>D3*Prices!$B2*Taxes!$B2+D4*Prices!$B3*Taxes!$B3+D5*Prices!$B4*Taxes!$B4+D6*Prices!$B5*Taxes!$B5</f>
         <v>141941.25</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <f>E3*Prices!$B2*Taxes!$B2+E4*Prices!$B3*Taxes!$B3+E5*Prices!$B4*Taxes!$B4+E6*Prices!$B5*Taxes!$B5</f>
         <v>153991.25</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12">
+      <c r="F8" s="10"/>
+      <c r="G8" s="11">
         <f>SUM(G3:G6)</f>
         <v>545393.75</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="11">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10">
         <f>B7*Taxes!$B8</f>
         <v>259770</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <f>C7*Taxes!$B8</f>
         <v>262185</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <f>D7*Taxes!$B8</f>
         <v>317835</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <f>E7*Taxes!$B8</f>
         <v>313635</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11">
         <f>SUM(H3:H6)</f>
         <v>1153425</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="13">
+        <v>12</v>
+      </c>
+      <c r="B10" s="12">
         <f>SUM(B7:B9)</f>
         <v>1626127.5</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <f t="shared" ref="C10:E10" si="1">SUM(C7:C9)</f>
         <v>1630788.75</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <f t="shared" si="1"/>
         <v>1973276.25</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <f t="shared" si="1"/>
         <v>1961126.25</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13">
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12">
         <f>SUM(I3:I6)</f>
         <v>7191318.75</v>
       </c>
@@ -1375,60 +1375,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>13</v>
+      <c r="F2" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <f>'Madrid-Solution'!F3</f>
         <v>1005000</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <f>'Barcelona-Solution'!F3</f>
         <v>825000</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <f>'Sevilla-Solution'!F3</f>
         <v>1020000</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <f>'Valencia-Solution'!F3</f>
         <v>825000</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <f>SUM(B3:E3)</f>
         <v>3675000</v>
       </c>
@@ -1437,23 +1437,23 @@
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <f>'Madrid-Solution'!F4</f>
         <v>910000</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <f>'Barcelona-Solution'!F4</f>
         <v>1190000</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <f>'Sevilla-Solution'!F4</f>
         <v>770000</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <f>'Valencia-Solution'!F4</f>
         <v>805000</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <f t="shared" ref="F4:F6" si="0">SUM(B4:E4)</f>
         <v>3675000</v>
       </c>
@@ -1462,148 +1462,148 @@
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <f>'Madrid-Solution'!F5</f>
         <v>3465000</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <f>'Barcelona-Solution'!F5</f>
         <v>2856000</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <f>'Sevilla-Solution'!F5</f>
         <v>1701000</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <f>'Valencia-Solution'!F5</f>
         <v>3255000</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f t="shared" si="0"/>
         <v>11277000</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="12">
+        <v>24</v>
+      </c>
+      <c r="B6" s="11">
         <f>'Madrid-Solution'!F6</f>
         <v>322500</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <f>'Barcelona-Solution'!F6</f>
         <v>127500</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <f>'Sevilla-Solution'!F6</f>
         <v>210000</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <f>'Valencia-Solution'!F6</f>
         <v>607500</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <f t="shared" si="0"/>
         <v>1267500</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="11">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10">
         <f>SUM(B3:B6)</f>
         <v>5702500</v>
       </c>
-      <c r="C7" s="11">
-        <f t="shared" ref="C7:F7" si="1">SUM(C3:C6)</f>
+      <c r="C7" s="10">
+        <f t="shared" ref="C7:E7" si="1">SUM(C3:C6)</f>
         <v>4998500</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <f t="shared" si="1"/>
         <v>3701000</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <f t="shared" si="1"/>
         <v>5492500</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <f>SUM(B7:E7)</f>
         <v>19894500</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="11">
+        <v>14</v>
+      </c>
+      <c r="B8" s="10">
         <f>'Madrid-Solution'!G8</f>
         <v>585368.75</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <f>'Barcelona-Solution'!G8</f>
         <v>540478.75</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <f>'Sevilla-Solution'!G8</f>
         <v>388847.5</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <f>'Valencia-Solution'!G8</f>
         <v>545393.75</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f>SUM(B8:E8)</f>
         <v>2060088.75</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="11">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10">
         <f>'Madrid-Solution'!H9</f>
         <v>1197525</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <f>'Barcelona-Solution'!H9</f>
         <v>1049685</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <f>'Sevilla-Solution'!H9</f>
         <v>777210</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <f>'Valencia-Solution'!H9</f>
         <v>1153425</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <f>SUM(B9:E9)</f>
         <v>4177845</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="13">
+        <v>12</v>
+      </c>
+      <c r="B10" s="12">
         <f>SUM(B7:B9)</f>
         <v>7485393.75</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <f t="shared" ref="C10:F10" si="2">SUM(C7:C9)</f>
         <v>6588663.75</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <f t="shared" si="2"/>
         <v>4867057.5</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <f t="shared" si="2"/>
         <v>7191318.75</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <f t="shared" si="2"/>
         <v>26132433.75</v>
       </c>
@@ -1623,55 +1623,55 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" activeCellId="1" sqref="F3:I10 B7:E10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="A1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1690,10 +1690,10 @@
       <c r="E3" s="4">
         <v>14</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -1711,10 +1711,10 @@
       <c r="E4" s="5">
         <v>12</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1732,14 +1732,14 @@
       <c r="E5" s="5">
         <v>32</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7">
         <v>5</v>
@@ -1753,62 +1753,62 @@
       <c r="E6" s="7">
         <v>2</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+        <v>14</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="18"/>
+        <v>10</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
+        <v>12</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1829,7 +1829,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -1838,43 +1838,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="A1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1893,10 +1893,10 @@
       <c r="E3" s="4">
         <v>11</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -1914,10 +1914,10 @@
       <c r="E4" s="5">
         <v>5</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1935,14 +1935,14 @@
       <c r="E5" s="5">
         <v>15</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7">
         <v>6</v>
@@ -1956,62 +1956,62 @@
       <c r="E6" s="7">
         <v>3</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+        <v>14</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="18"/>
+        <v>10</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
+        <v>12</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2032,50 +2032,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="A1" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2094,10 +2094,10 @@
       <c r="E3" s="4">
         <v>16</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -2115,10 +2115,10 @@
       <c r="E4" s="5">
         <v>8</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2136,14 +2136,14 @@
       <c r="E5" s="5">
         <v>41</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7">
         <v>14</v>
@@ -2157,62 +2157,62 @@
       <c r="E6" s="7">
         <v>15</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+        <v>14</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="18"/>
+        <v>10</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
+        <v>12</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2233,118 +2233,118 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>13</v>
+      <c r="F2" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
+        <v>24</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
+        <v>14</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
+        <v>10</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+        <v>12</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2365,13 +2365,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2400,7 +2400,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1">
         <v>7500</v>
@@ -2417,18 +2417,18 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2457,7 +2457,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B5" s="3">
         <v>4.7500000000000001E-2</v>
@@ -2465,7 +2465,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3">
         <v>0.21</v>
@@ -2486,50 +2486,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2548,19 +2548,19 @@
       <c r="E3" s="4">
         <v>12</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <f>SUM(B3:E3)*Prices!B2</f>
         <v>1005000</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <f>F3*Taxes!B2</f>
         <v>97987.5</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <f>F3*Taxes!B$8</f>
         <v>211050</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="9">
         <f>SUM(F3:H3)</f>
         <v>1314037.5</v>
       </c>
@@ -2581,19 +2581,19 @@
       <c r="E4" s="5">
         <v>8</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <f>SUM(B4:E4)*Prices!B3</f>
         <v>910000</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <f>F4*Taxes!B3</f>
         <v>134225</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <f>F4*Taxes!B$8</f>
         <v>191100</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="10">
         <f t="shared" ref="I4:I6" si="0">SUM(F4:H4)</f>
         <v>1235325</v>
       </c>
@@ -2614,26 +2614,26 @@
       <c r="E5" s="5">
         <v>30</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f>SUM(B5:E5)*Prices!B4</f>
         <v>3465000</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <f>F5*Taxes!B4</f>
         <v>337837.5</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <f>F5*Taxes!B$8</f>
         <v>727650</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <f t="shared" si="0"/>
         <v>4530487.5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7">
         <v>10</v>
@@ -2647,131 +2647,131 @@
       <c r="E6" s="7">
         <v>6</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f>SUM(B6:E6)*Prices!B5</f>
         <v>322500</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <f>F6*Taxes!B5</f>
         <v>15318.75</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f>F6*Taxes!B$8</f>
         <v>67725</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <f t="shared" si="0"/>
         <v>405543.75</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="11">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10">
         <f>B3*Prices!$B2+B4*Prices!$B3+B5*Prices!$B4+B6*Prices!$B5</f>
         <v>1600000</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <f>C3*Prices!$B2+C4*Prices!$B3+C5*Prices!$B4+C6*Prices!$B5</f>
         <v>1388000</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <f>D3*Prices!$B2+D4*Prices!$B3+D5*Prices!$B4+D6*Prices!$B5</f>
         <v>1579500</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <f>E3*Prices!$B2+E4*Prices!$B3+E5*Prices!$B4+E6*Prices!$B5</f>
         <v>1135000</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <f>SUM(F3:F6)</f>
         <v>5702500</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="11">
+        <v>14</v>
+      </c>
+      <c r="B8" s="10">
         <f>B3*Prices!$B2*Taxes!$B2+B4*Prices!$B3*Taxes!$B3+B5*Prices!$B4*Taxes!$B4+B6*Prices!$B5*Taxes!$B5</f>
         <v>166250</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <f>C3*Prices!$B2*Taxes!$B2+C4*Prices!$B3*Taxes!$B3+C5*Prices!$B4*Taxes!$B4+C6*Prices!$B5*Taxes!$B5</f>
         <v>143080</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <f>D3*Prices!$B2*Taxes!$B2+D4*Prices!$B3*Taxes!$B3+D5*Prices!$B4*Taxes!$B4+D6*Prices!$B5*Taxes!$B5</f>
         <v>153626.25</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <f>E3*Prices!$B2*Taxes!$B2+E4*Prices!$B3*Taxes!$B3+E5*Prices!$B4*Taxes!$B4+E6*Prices!$B5*Taxes!$B5</f>
         <v>122412.5</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12">
+      <c r="F8" s="10"/>
+      <c r="G8" s="11">
         <f>SUM(G3:G6)</f>
         <v>585368.75</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="11">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10">
         <f>B7*Taxes!$B8</f>
         <v>336000</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <f>C7*Taxes!$B8</f>
         <v>291480</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <f>D7*Taxes!$B8</f>
         <v>331695</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <f>E7*Taxes!$B8</f>
         <v>238350</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11">
         <f>SUM(H3:H6)</f>
         <v>1197525</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="13">
+        <v>12</v>
+      </c>
+      <c r="B10" s="12">
         <f>SUM(B7:B9)</f>
         <v>2102250</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <f t="shared" ref="C10:E10" si="1">SUM(C7:C9)</f>
         <v>1822560</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <f t="shared" si="1"/>
         <v>2064821.25</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <f t="shared" si="1"/>
         <v>1495762.5</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13">
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12">
         <f>SUM(I3:I6)</f>
         <v>7485393.75</v>
       </c>
@@ -2796,50 +2796,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="A1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2858,19 +2858,19 @@
       <c r="E3" s="4">
         <v>14</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <f>SUM(B3:E3)*Prices!B2</f>
         <v>825000</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <f>F3*Taxes!B2</f>
         <v>80437.5</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <f>F3*Taxes!B$8</f>
         <v>173250</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="9">
         <f>SUM(F3:H3)</f>
         <v>1078687.5</v>
       </c>
@@ -2891,19 +2891,19 @@
       <c r="E4" s="5">
         <v>12</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <f>SUM(B4:E4)*Prices!B3</f>
         <v>1190000</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <f>F4*Taxes!B3</f>
         <v>175525</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <f>F4*Taxes!B$8</f>
         <v>249900</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="10">
         <f t="shared" ref="I4:I6" si="0">SUM(F4:H4)</f>
         <v>1615425</v>
       </c>
@@ -2924,26 +2924,26 @@
       <c r="E5" s="5">
         <v>32</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f>SUM(B5:E5)*Prices!B4</f>
         <v>2856000</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <f>F5*Taxes!B4</f>
         <v>278460</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <f>F5*Taxes!B$8</f>
         <v>599760</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <f t="shared" si="0"/>
         <v>3734220</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7">
         <v>5</v>
@@ -2957,131 +2957,131 @@
       <c r="E6" s="7">
         <v>2</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f>SUM(B6:E6)*Prices!B5</f>
         <v>127500</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <f>F6*Taxes!B5</f>
         <v>6056.25</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f>F6*Taxes!B$8</f>
         <v>26775</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <f t="shared" si="0"/>
         <v>160331.25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="11">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10">
         <f>B3*Prices!$B2+B4*Prices!$B3+B5*Prices!$B4+B6*Prices!$B5</f>
         <v>1036500</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <f>C3*Prices!$B2+C4*Prices!$B3+C5*Prices!$B4+C6*Prices!$B5</f>
         <v>1172500</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <f>D3*Prices!$B2+D4*Prices!$B3+D5*Prices!$B4+D6*Prices!$B5</f>
         <v>1472500</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <f>E3*Prices!$B2+E4*Prices!$B3+E5*Prices!$B4+E6*Prices!$B5</f>
         <v>1317000</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <f>SUM(F3:F6)</f>
         <v>4998500</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="11">
+        <v>14</v>
+      </c>
+      <c r="B8" s="10">
         <f>B3*Prices!$B2*Taxes!$B2+B4*Prices!$B3*Taxes!$B3+B5*Prices!$B4*Taxes!$B4+B6*Prices!$B5*Taxes!$B5</f>
         <v>114933.75</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <f>C3*Prices!$B2*Taxes!$B2+C4*Prices!$B3*Taxes!$B3+C5*Prices!$B4*Taxes!$B4+C6*Prices!$B5*Taxes!$B5</f>
         <v>127193.75</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <f>D3*Prices!$B2*Taxes!$B2+D4*Prices!$B3*Taxes!$B3+D5*Prices!$B4*Taxes!$B4+D6*Prices!$B5*Taxes!$B5</f>
         <v>149693.75</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <f>E3*Prices!$B2*Taxes!$B2+E4*Prices!$B3*Taxes!$B3+E5*Prices!$B4*Taxes!$B4+E6*Prices!$B5*Taxes!$B5</f>
         <v>148657.5</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12">
+      <c r="F8" s="10"/>
+      <c r="G8" s="11">
         <f>SUM(G3:G6)</f>
         <v>540478.75</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="11">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10">
         <f>B7*Taxes!$B8</f>
         <v>217665</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <f>C7*Taxes!$B8</f>
         <v>246225</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <f>D7*Taxes!$B8</f>
         <v>309225</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <f>E7*Taxes!$B8</f>
         <v>276570</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11">
         <f>SUM(H3:H6)</f>
         <v>1049685</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="13">
+        <v>12</v>
+      </c>
+      <c r="B10" s="12">
         <f>SUM(B7:B9)</f>
         <v>1369098.75</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <f t="shared" ref="C10:E10" si="1">SUM(C7:C9)</f>
         <v>1545918.75</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <f t="shared" si="1"/>
         <v>1931418.75</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <f t="shared" si="1"/>
         <v>1742227.5</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13">
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12">
         <f>SUM(I3:I6)</f>
         <v>6588663.75</v>
       </c>

</xml_diff>